<commit_message>
Bunch of test cases
</commit_message>
<xml_diff>
--- a/documentation/sprint 4/Sprint 4 Tests.xlsx
+++ b/documentation/sprint 4/Sprint 4 Tests.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75D2BE76-6230-4F12-8454-01603FD61B74}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564053C2-05E6-4BA7-B855-0C97B3A22B57}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Test</t>
   </si>
@@ -35,6 +35,177 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Adds green if match or red if doesn’t match</t>
+  </si>
+  <si>
+    <t>Matching predicted with actual result for 2016</t>
+  </si>
+  <si>
+    <t>Returned red when it should return green</t>
+  </si>
+  <si>
+    <t>Outcomes csv was formatted wrong, changed the formatting</t>
+  </si>
+  <si>
+    <t>Matching predicted with actual result for 14&amp;15</t>
+  </si>
+  <si>
+    <t>Out of length error</t>
+  </si>
+  <si>
+    <t>Returned the outcomes without names, and prediction without names</t>
+  </si>
+  <si>
+    <t>Displaying points and % games on site</t>
+  </si>
+  <si>
+    <t>Display correct info in label</t>
+  </si>
+  <si>
+    <t>Showed a tuple instead of a single value</t>
+  </si>
+  <si>
+    <t>Passed in first index instead of full value</t>
+  </si>
+  <si>
+    <t>Reading scores files</t>
+  </si>
+  <si>
+    <t>Parsing Scores files</t>
+  </si>
+  <si>
+    <t>Comparing scores to predicted score</t>
+  </si>
+  <si>
+    <t>Formatting output string</t>
+  </si>
+  <si>
+    <t>Formatting full output array</t>
+  </si>
+  <si>
+    <t>Sorting Arrays</t>
+  </si>
+  <si>
+    <t>Writing Output into Bucket manually</t>
+  </si>
+  <si>
+    <t>Writing output automatically from website</t>
+  </si>
+  <si>
+    <t>Displaying the high scores in HTML</t>
+  </si>
+  <si>
+    <t>Linking home page to high score page</t>
+  </si>
+  <si>
+    <t>Updating high scores</t>
+  </si>
+  <si>
+    <t>Gets the full data from the file</t>
+  </si>
+  <si>
+    <t>splits the file into each of the scores</t>
+  </si>
+  <si>
+    <t>indexes through each score and checks if our score is greater</t>
+  </si>
+  <si>
+    <t>Correctly built string</t>
+  </si>
+  <si>
+    <t>Output Array writes in a logical format</t>
+  </si>
+  <si>
+    <t>output array writes into a logical format</t>
+  </si>
+  <si>
+    <t>returns scores in ascending order</t>
+  </si>
+  <si>
+    <t>data shows up in file on bucket</t>
+  </si>
+  <si>
+    <t>each score element displays correctly into the table</t>
+  </si>
+  <si>
+    <t>high scores button links to high score url</t>
+  </si>
+  <si>
+    <t>After making a new high score, page auto updates</t>
+  </si>
+  <si>
+    <t>File not found in bucket</t>
+  </si>
+  <si>
+    <t>Split the file into each part of the score, instead of full scores</t>
+  </si>
+  <si>
+    <t>Skipped all if statements when they should have matched</t>
+  </si>
+  <si>
+    <t>String added an extra "|" at the end</t>
+  </si>
+  <si>
+    <t>Output array writes blank</t>
+  </si>
+  <si>
+    <t>output array was difficult to parse back when needed</t>
+  </si>
+  <si>
+    <t>returns scores random order</t>
+  </si>
+  <si>
+    <t>Data didn’t write at all</t>
+  </si>
+  <si>
+    <t>Data didn't write for several minutes after</t>
+  </si>
+  <si>
+    <t>Scores were split every char instead of at spaces</t>
+  </si>
+  <si>
+    <t>URL NOT FOUND</t>
+  </si>
+  <si>
+    <t>Scores would not update until a re-deploy</t>
+  </si>
+  <si>
+    <t>Made score files public</t>
+  </si>
+  <si>
+    <t>split on '|' instead of default</t>
+  </si>
+  <si>
+    <t>cast the year to an int</t>
+  </si>
+  <si>
+    <t>deleted extra "|"</t>
+  </si>
+  <si>
+    <t>Passed in correct output instead of a blank array</t>
+  </si>
+  <si>
+    <t>Reformatted the output to be clearly seperated</t>
+  </si>
+  <si>
+    <t>Used sorted() instead of list.sort</t>
+  </si>
+  <si>
+    <t>Allowed write access to file</t>
+  </si>
+  <si>
+    <t>Changed the writing format, still slow, but slightly faster</t>
+  </si>
+  <si>
+    <t>added split at " " instead of ""</t>
+  </si>
+  <si>
+    <t>Defined the url in urls.py</t>
+  </si>
+  <si>
+    <t>Added line the reread the file each time the button was clicked</t>
   </si>
 </sst>
 </file>
@@ -376,20 +547,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.20703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,64 +577,274 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3">
+        <v>43216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="3">
+        <v>43217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="3">
+        <v>43217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3">
+        <v>43218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="3">
+        <v>43218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="3">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="3">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="3">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="3"/>
     </row>
   </sheetData>

</xml_diff>